<commit_message>
Moved Pending Rollovers out of Preprocessing and into main part of the program. Added handling of the information from the pending rollovers file. Added sheet to Payout Prototype for Pending Rollovers. Added logic to add pending rollover items that are ready to move on into ynm and yne financial information
</commit_message>
<xml_diff>
--- a/YNM Payout Prototype.xlsx
+++ b/YNM Payout Prototype.xlsx
@@ -13,6 +13,7 @@
     <sheet name="YNE Collab Payouts" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Combined Payouts" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Combined Next Month Rollovers" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Pending Rollovers" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2899,7 +2900,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2912,7 +2913,7 @@
     <col width="19" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="16" customWidth="1" min="5" max="5"/>
-    <col width="6" customWidth="1" min="6" max="6"/>
+    <col width="7" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
@@ -3098,12 +3099,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Lifelinelemons</t>
+          <t>Bermuda</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lifelinelemons Candy Girls 3' Charms</t>
+          <t>Bermuda Muda Bellypad</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3112,25 +3113,25 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>39.15</v>
+        <v>1401.05</v>
       </c>
       <c r="E7" t="n">
-        <v>1.17</v>
+        <v>42.03</v>
       </c>
       <c r="F7" t="n">
-        <v>9</v>
+        <v>560</v>
       </c>
       <c r="G7" t="n">
-        <v>28.98</v>
+        <v>799.02</v>
       </c>
       <c r="H7" t="n">
-        <v>11.592</v>
+        <v>319.608</v>
       </c>
       <c r="I7" t="n">
-        <v>14.49</v>
+        <v>399.51</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>17.388</v>
+        <v>479.412</v>
       </c>
     </row>
     <row r="8">
@@ -3140,7 +3141,7 @@
         </is>
       </c>
       <c r="J8" s="4" t="n">
-        <v>17.388</v>
+        <v>479.412</v>
       </c>
     </row>
     <row r="9">
@@ -3210,162 +3211,162 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Lifelinelemons</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Lifelinelemons Candy Girls 3' Charms</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>39.15</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="F11" t="n">
+        <v>9</v>
+      </c>
+      <c r="G11" t="n">
+        <v>28.98</v>
+      </c>
+      <c r="H11" t="n">
+        <v>11.592</v>
+      </c>
+      <c r="I11" t="n">
+        <v>14.49</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>17.388</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="I12" s="4" t="inlineStr">
+        <is>
+          <t>Total Payout</t>
+        </is>
+      </c>
+      <c r="J12" s="4" t="n">
+        <v>17.388</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n"/>
+      <c r="B13" s="1" t="n"/>
+      <c r="C13" s="1" t="n"/>
+      <c r="D13" s="1" t="n"/>
+      <c r="E13" s="1" t="n"/>
+      <c r="F13" s="1" t="n"/>
+      <c r="G13" s="1" t="n"/>
+      <c r="H13" s="1" t="n"/>
+      <c r="I13" s="1" t="n"/>
+      <c r="J13" s="1" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Artist Name</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>Distribution Type</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>Total Value</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>Processing Fee</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+      <c r="G14" s="2" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+      <c r="H14" s="2" t="inlineStr">
+        <is>
+          <t>SPE 40%</t>
+        </is>
+      </c>
+      <c r="I14" s="2" t="inlineStr">
+        <is>
+          <t>SPE 50%</t>
+        </is>
+      </c>
+      <c r="J14" s="2" t="inlineStr">
+        <is>
+          <t>SPE 60%</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>Maxiebreak</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>X-BurgerG0dde55_Xx Photocard Set</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>Original</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D15" t="n">
         <v>52.2</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E15" t="n">
         <v>1.57</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F15" t="n">
         <v>15</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G15" t="n">
         <v>35.63</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H15" t="n">
         <v>14.252</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I15" t="n">
         <v>17.815</v>
       </c>
-      <c r="J11" s="3" t="n">
+      <c r="J15" s="3" t="n">
         <v>21.378</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Maxiebreak</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Wide Load Bumper Stickers</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Original</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>41.76</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="F12" t="n">
-        <v>12</v>
-      </c>
-      <c r="G12" t="n">
-        <v>28.51</v>
-      </c>
-      <c r="H12" t="n">
-        <v>11.404</v>
-      </c>
-      <c r="I12" t="n">
-        <v>14.255</v>
-      </c>
-      <c r="J12" s="3" t="n">
-        <v>17.106</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="I13" s="4" t="inlineStr">
-        <is>
-          <t>Total Payout</t>
-        </is>
-      </c>
-      <c r="J13" s="4" t="n">
-        <v>38.48399999999999</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n"/>
-      <c r="B14" s="1" t="n"/>
-      <c r="C14" s="1" t="n"/>
-      <c r="D14" s="1" t="n"/>
-      <c r="E14" s="1" t="n"/>
-      <c r="F14" s="1" t="n"/>
-      <c r="G14" s="1" t="n"/>
-      <c r="H14" s="1" t="n"/>
-      <c r="I14" s="1" t="n"/>
-      <c r="J14" s="1" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>Artist Name</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>Item</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="inlineStr">
-        <is>
-          <t>Distribution Type</t>
-        </is>
-      </c>
-      <c r="D15" s="2" t="inlineStr">
-        <is>
-          <t>Total Value</t>
-        </is>
-      </c>
-      <c r="E15" s="2" t="inlineStr">
-        <is>
-          <t>Processing Fee</t>
-        </is>
-      </c>
-      <c r="F15" s="2" t="inlineStr">
-        <is>
-          <t>Cost</t>
-        </is>
-      </c>
-      <c r="G15" s="2" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="H15" s="2" t="inlineStr">
-        <is>
-          <t>SPE 40%</t>
-        </is>
-      </c>
-      <c r="I15" s="2" t="inlineStr">
-        <is>
-          <t>SPE 50%</t>
-        </is>
-      </c>
-      <c r="J15" s="2" t="inlineStr">
-        <is>
-          <t>SPE 60%</t>
-        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Mintrimo</t>
+          <t>Maxiebreak</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Eleanor Standee</t>
+          <t>Wide Load Bumper Stickers</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -3374,25 +3375,25 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>26.1</v>
+        <v>41.76</v>
       </c>
       <c r="E16" t="n">
-        <v>0.78</v>
+        <v>1.25</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G16" t="n">
-        <v>25.32</v>
+        <v>28.51</v>
       </c>
       <c r="H16" t="n">
-        <v>10.128</v>
+        <v>11.404</v>
       </c>
       <c r="I16" t="n">
-        <v>12.66</v>
+        <v>14.255</v>
       </c>
       <c r="J16" s="3" t="n">
-        <v>15.192</v>
+        <v>17.106</v>
       </c>
     </row>
     <row r="17">
@@ -3402,7 +3403,7 @@
         </is>
       </c>
       <c r="J17" s="4" t="n">
-        <v>15.192</v>
+        <v>38.48399999999999</v>
       </c>
     </row>
     <row r="18">
@@ -3472,12 +3473,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Rattie</t>
+          <t>Mintrimo</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Retro Rat Sticker</t>
+          <t>Eleanor Standee</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -3486,25 +3487,25 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>5.22</v>
+        <v>26.1</v>
       </c>
       <c r="E20" t="n">
-        <v>0.16</v>
+        <v>0.78</v>
       </c>
       <c r="F20" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>3.56</v>
+        <v>25.32</v>
       </c>
       <c r="H20" t="n">
-        <v>1.424</v>
+        <v>10.128</v>
       </c>
       <c r="I20" t="n">
-        <v>1.78</v>
+        <v>12.66</v>
       </c>
       <c r="J20" s="3" t="n">
-        <v>2.136</v>
+        <v>15.192</v>
       </c>
     </row>
     <row r="21">
@@ -3514,7 +3515,7 @@
         </is>
       </c>
       <c r="J21" s="4" t="n">
-        <v>2.136</v>
+        <v>15.192</v>
       </c>
     </row>
     <row r="22">
@@ -3584,162 +3585,162 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>Rattie</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Retro Rat Sticker</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.424</v>
+      </c>
+      <c r="I24" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="J24" s="3" t="n">
+        <v>2.136</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="I25" s="4" t="inlineStr">
+        <is>
+          <t>Total Payout</t>
+        </is>
+      </c>
+      <c r="J25" s="4" t="n">
+        <v>2.136</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n"/>
+      <c r="B26" s="1" t="n"/>
+      <c r="C26" s="1" t="n"/>
+      <c r="D26" s="1" t="n"/>
+      <c r="E26" s="1" t="n"/>
+      <c r="F26" s="1" t="n"/>
+      <c r="G26" s="1" t="n"/>
+      <c r="H26" s="1" t="n"/>
+      <c r="I26" s="1" t="n"/>
+      <c r="J26" s="1" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>Artist Name</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="inlineStr">
+        <is>
+          <t>Distribution Type</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>Total Value</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>Processing Fee</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+      <c r="G27" s="2" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+      <c r="H27" s="2" t="inlineStr">
+        <is>
+          <t>SPE 40%</t>
+        </is>
+      </c>
+      <c r="I27" s="2" t="inlineStr">
+        <is>
+          <t>SPE 50%</t>
+        </is>
+      </c>
+      <c r="J27" s="2" t="inlineStr">
+        <is>
+          <t>SPE 60%</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Skullgeist</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B28" t="inlineStr">
         <is>
           <t>Iconic Plant Girl (Standee)</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>Original</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="D28" t="n">
         <v>26.1</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E28" t="n">
         <v>0.78</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F28" t="n">
         <v>10</v>
       </c>
-      <c r="G24" t="n">
+      <c r="G28" t="n">
         <v>15.32</v>
       </c>
-      <c r="H24" t="n">
+      <c r="H28" t="n">
         <v>6.128</v>
       </c>
-      <c r="I24" t="n">
+      <c r="I28" t="n">
         <v>7.66</v>
       </c>
-      <c r="J24" s="3" t="n">
+      <c r="J28" s="3" t="n">
         <v>9.192</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Skullgeist</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Iconic Plant Girl Sticker</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Original</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>10</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="F25" t="n">
-        <v>3</v>
-      </c>
-      <c r="G25" t="n">
-        <v>6.699999999999999</v>
-      </c>
-      <c r="H25" t="n">
-        <v>2.68</v>
-      </c>
-      <c r="I25" t="n">
-        <v>3.35</v>
-      </c>
-      <c r="J25" s="3" t="n">
-        <v>4.02</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="I26" s="4" t="inlineStr">
-        <is>
-          <t>Total Payout</t>
-        </is>
-      </c>
-      <c r="J26" s="4" t="n">
-        <v>13.212</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n"/>
-      <c r="B27" s="1" t="n"/>
-      <c r="C27" s="1" t="n"/>
-      <c r="D27" s="1" t="n"/>
-      <c r="E27" s="1" t="n"/>
-      <c r="F27" s="1" t="n"/>
-      <c r="G27" s="1" t="n"/>
-      <c r="H27" s="1" t="n"/>
-      <c r="I27" s="1" t="n"/>
-      <c r="J27" s="1" t="n"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="inlineStr">
-        <is>
-          <t>Artist Name</t>
-        </is>
-      </c>
-      <c r="B28" s="2" t="inlineStr">
-        <is>
-          <t>Item</t>
-        </is>
-      </c>
-      <c r="C28" s="2" t="inlineStr">
-        <is>
-          <t>Distribution Type</t>
-        </is>
-      </c>
-      <c r="D28" s="2" t="inlineStr">
-        <is>
-          <t>Total Value</t>
-        </is>
-      </c>
-      <c r="E28" s="2" t="inlineStr">
-        <is>
-          <t>Processing Fee</t>
-        </is>
-      </c>
-      <c r="F28" s="2" t="inlineStr">
-        <is>
-          <t>Cost</t>
-        </is>
-      </c>
-      <c r="G28" s="2" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="H28" s="2" t="inlineStr">
-        <is>
-          <t>SPE 40%</t>
-        </is>
-      </c>
-      <c r="I28" s="2" t="inlineStr">
-        <is>
-          <t>SPE 50%</t>
-        </is>
-      </c>
-      <c r="J28" s="2" t="inlineStr">
-        <is>
-          <t>SPE 60%</t>
-        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Waifudekai</t>
+          <t>Skullgeist</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Fat Girl Fall Purin 11x17 Print [PURINTOBER CHARITY]</t>
+          <t>Iconic Plant Girl Sticker</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -3748,25 +3749,25 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>20.88</v>
+        <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>0.63</v>
+        <v>0.3</v>
       </c>
       <c r="F29" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="G29" t="n">
-        <v>16.75</v>
+        <v>6.699999999999999</v>
       </c>
       <c r="H29" t="n">
-        <v>6.7</v>
+        <v>2.68</v>
       </c>
       <c r="I29" t="n">
-        <v>8.375</v>
+        <v>3.35</v>
       </c>
       <c r="J29" s="3" t="n">
-        <v>10.05</v>
+        <v>4.02</v>
       </c>
     </row>
     <row r="30">
@@ -3776,6 +3777,118 @@
         </is>
       </c>
       <c r="J30" s="4" t="n">
+        <v>13.212</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n"/>
+      <c r="B31" s="1" t="n"/>
+      <c r="C31" s="1" t="n"/>
+      <c r="D31" s="1" t="n"/>
+      <c r="E31" s="1" t="n"/>
+      <c r="F31" s="1" t="n"/>
+      <c r="G31" s="1" t="n"/>
+      <c r="H31" s="1" t="n"/>
+      <c r="I31" s="1" t="n"/>
+      <c r="J31" s="1" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>Artist Name</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
+          <t>Distribution Type</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>Total Value</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>Processing Fee</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+      <c r="G32" s="2" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+      <c r="H32" s="2" t="inlineStr">
+        <is>
+          <t>SPE 40%</t>
+        </is>
+      </c>
+      <c r="I32" s="2" t="inlineStr">
+        <is>
+          <t>SPE 50%</t>
+        </is>
+      </c>
+      <c r="J32" s="2" t="inlineStr">
+        <is>
+          <t>SPE 60%</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Waifudekai</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Fat Girl Fall Purin 11x17 Print [PURINTOBER CHARITY]</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>20.88</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="F33" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G33" t="n">
+        <v>16.75</v>
+      </c>
+      <c r="H33" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="I33" t="n">
+        <v>8.375</v>
+      </c>
+      <c r="J33" s="3" t="n">
+        <v>10.05</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="I34" s="4" t="inlineStr">
+        <is>
+          <t>Total Payout</t>
+        </is>
+      </c>
+      <c r="J34" s="4" t="n">
         <v>10.05</v>
       </c>
     </row>
@@ -3966,7 +4079,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8.890000000000001</v>
+        <v>488.3</v>
       </c>
     </row>
     <row r="11">
@@ -5419,4 +5532,109 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>Origin</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Artist</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>Distribution Type</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>Total Value</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>Processing Fee</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>Ready</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>YNE</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>KafeKafei</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Moomochi 3D Belly Mousepad (PRE-ORDER)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>250</v>
+      </c>
+      <c r="F2" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="G2" t="n">
+        <v>100</v>
+      </c>
+      <c r="H2" t="n">
+        <v>142.5</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>